<commit_message>
Added proper comment in Write_data_to_csc file
</commit_message>
<xml_diff>
--- a/PIPAssignment1/DataFile/Employe1.xlsx
+++ b/PIPAssignment1/DataFile/Employe1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>salamna</t>
   </si>
@@ -80,6 +80,24 @@
   </si>
   <si>
     <t>sdet1</t>
+  </si>
+  <si>
+    <t>salmanalam</t>
+  </si>
+  <si>
+    <t>543262</t>
+  </si>
+  <si>
+    <t>Devops</t>
+  </si>
+  <si>
+    <t>farmankhan</t>
+  </si>
+  <si>
+    <t>345672</t>
+  </si>
+  <si>
+    <t>Ba</t>
   </si>
 </sst>
 </file>
@@ -584,6 +602,34 @@
         <v>14</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added proper comment in Update_detail file
</commit_message>
<xml_diff>
--- a/PIPAssignment1/DataFile/Employe1.xlsx
+++ b/PIPAssignment1/DataFile/Employe1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
   <si>
     <t>salamna</t>
   </si>
@@ -624,7 +624,7 @@
         <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Added proper comment in Patter_match file and modify the excel file data.
</commit_message>
<xml_diff>
--- a/PIPAssignment1/DataFile/Employe1.xlsx
+++ b/PIPAssignment1/DataFile/Employe1.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mumarkhan\eclipse-workspace\Ruby_Project_list\Assignmentpip\DataFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mumarkhan\eclipse-workspace\PIPAssignment\PIPAssignment1\DataFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBA3597-4952-47E6-8C39-635FB420C72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001DB1AE-0022-4A39-8679-F17831D7EB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,26 +20,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>salamna</t>
   </si>
   <si>
-    <t>09654</t>
-  </si>
-  <si>
     <t>QA</t>
   </si>
   <si>
     <t>m</t>
   </si>
   <si>
-    <t>sofiya</t>
-  </si>
-  <si>
-    <t>342524</t>
-  </si>
-  <si>
     <t>f</t>
   </si>
   <si>
@@ -58,12 +49,6 @@
     <t>Arshiybano</t>
   </si>
   <si>
-    <t>98765</t>
-  </si>
-  <si>
-    <t>BA</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -73,9 +58,6 @@
     <t>SDET2</t>
   </si>
   <si>
-    <t>SDET3</t>
-  </si>
-  <si>
     <t>DEVOPS</t>
   </si>
   <si>
@@ -85,27 +67,38 @@
     <t>salmanalam</t>
   </si>
   <si>
-    <t>543262</t>
-  </si>
-  <si>
     <t>Devops</t>
   </si>
   <si>
     <t>farmankhan</t>
   </si>
   <si>
-    <t>345672</t>
-  </si>
-  <si>
-    <t>Ba</t>
+    <t>sofiyaansari</t>
+  </si>
+  <si>
+    <t>Saniya khan</t>
+  </si>
+  <si>
+    <t>sanakhan</t>
+  </si>
+  <si>
+    <t>salamnakhan</t>
+  </si>
+  <si>
+    <t>sofiyaalam</t>
+  </si>
+  <si>
+    <t>Maaz</t>
+  </si>
+  <si>
+    <t>Vidhi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -450,55 +443,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="19.36328125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.54296875" collapsed="true"/>
+    <col min="2" max="2" width="19.36328125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.54296875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>12346</v>
+      </c>
+      <c r="C3" t="s">
         <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -506,13 +499,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>12347</v>
+      </c>
+      <c r="C4" t="s">
         <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -522,112 +515,112 @@
       <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>96540</v>
+      </c>
+      <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>96542</v>
+      </c>
+      <c r="C6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>34200</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>9054</v>
+      </c>
+      <c r="C8" t="s">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>302504</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>987650</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>5432020</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>305672</v>
+      </c>
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>